<commit_message>
1. Reinitialised after source-id modified.
</commit_message>
<xml_diff>
--- a/cmip6/models/mri-esm2-0/cmip6_mri_mri-esm2-0_aerosol.xlsx
+++ b/cmip6/models/mri-esm2-0/cmip6_mri_mri-esm2-0_aerosol.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="506">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -162,7 +162,7 @@
     <t>cmip6.aerosol.key_properties.name</t>
   </si>
   <si>
-    <t>MASINGAR mk-2r4c</t>
+    <t>MASINGAR mk-2</t>
   </si>
   <si>
     <t>1.1.1.2 *</t>
@@ -195,9 +195,7 @@
     <t>NOTE: Double click to expand if text is too long for cell</t>
   </si>
   <si>
-    <t xml:space="preserve">Model of Aerosol Species in the Global Atmosphere mark-2 revision 4-climate (MASINGAR mk-2r4c) treats atmospheric aerosol physical and chemical processes (e.g., emission, transport, diffusion, chemical reactions, and dry and wet depositions) and includes the following species: non-sea-salt sulfate, black carbon, organic carbon, sea salt, mineral dust, and aerosol precursor gases (e.g., sulfur dioxide and dimethyl sulfide).
-References: Tanaka et al. 2003; Yukimoto et al. submitted; Oshima et al., in preparation
-</t>
+    <t>References: Yukimoto et al. 2011;Yukimoto et al. 2012; Adachi et al. 2013</t>
   </si>
   <si>
     <t>1.1.1.4 *</t>
@@ -332,9 +330,6 @@
     <t>cmip6.aerosol.key_properties.software_properties.code_version</t>
   </si>
   <si>
-    <t>masingar_mk2r4_ESM2</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.2.1.3 </t>
   </si>
   <si>
@@ -347,9 +342,6 @@
     <t>cmip6.aerosol.key_properties.software_properties.code_languages</t>
   </si>
   <si>
-    <t>Fortran 95</t>
-  </si>
-  <si>
     <t>1.3.1</t>
   </si>
   <si>
@@ -371,12 +363,15 @@
     <t>cmip6.aerosol.key_properties.timestep_framework.method</t>
   </si>
   <si>
+    <t>Other: specific time stepping (integrated)</t>
+  </si>
+  <si>
+    <t>Uses atmospheric chemistry time stepping</t>
+  </si>
+  <si>
     <t>Specific timestepping (operator splitting)</t>
   </si>
   <si>
-    <t>Uses atmospheric chemistry time stepping</t>
-  </si>
-  <si>
     <t>Specific timestepping (integrated)</t>
   </si>
   <si>
@@ -428,24 +423,24 @@
     <t>cmip6.aerosol.key_properties.timestep_framework.integrated_scheme_type</t>
   </si>
   <si>
+    <t>Explicit</t>
+  </si>
+  <si>
+    <t>Implicit</t>
+  </si>
+  <si>
+    <t>Semi-implicit</t>
+  </si>
+  <si>
+    <t>Semi-analytic</t>
+  </si>
+  <si>
+    <t>Impact solver</t>
+  </si>
+  <si>
     <t>Back Euler</t>
   </si>
   <si>
-    <t>Explicit</t>
-  </si>
-  <si>
-    <t>Implicit</t>
-  </si>
-  <si>
-    <t>Semi-implicit</t>
-  </si>
-  <si>
-    <t>Semi-analytic</t>
-  </si>
-  <si>
-    <t>Impact solver</t>
-  </si>
-  <si>
     <t>Newton Raphson</t>
   </si>
   <si>
@@ -470,10 +465,6 @@
     <t>cmip6.aerosol.key_properties.meteorological_forcings.variables_3D</t>
   </si>
   <si>
-    <t xml:space="preserve">U, V, T, Q, divergence, cloud droplet to rain conversion rate (convective cloud), cloud droplet to rain conversion rate (large-scale cloud), rain to vapor (convective cloud), rain to vapor (large-scale cloud), RH, organized entrainment rate, organized detrainment rate, upward mass flux in cumulus, cloud water content in cumulus, conversion from cloud water to precipitation in cumulus, cloud water content, cloud cover, eddy diffusion coefficient, ozone
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.4.1.2 </t>
   </si>
   <si>
@@ -486,9 +477,6 @@
     <t>cmip6.aerosol.key_properties.meteorological_forcings.variables_2D</t>
   </si>
   <si>
-    <t>SST, U(10m), V(10m), T(2m), Q(2m), zonal surface stress, meridional surface stress, friction velocity, sea ice fraction, roughness length, convective precipitation, large-scale precipitation, sensible heat flux, latent heat flux, ground temperature, snow cover, soil ice, vegetation cover (canopy), vegetation cover (grass), LAI (canopy), LAI (grass), volumetric soil water content, landmask type definitions, land-sea mask ratio, surface pressure, longitude derivative of surface pressure, latitude derivative of surface pressure</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.4.1.3 </t>
   </si>
   <si>
@@ -519,9 +507,6 @@
     <t>cmip6.aerosol.key_properties.resolution.name</t>
   </si>
   <si>
-    <t>TL95L80</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.5.1.2 </t>
   </si>
   <si>
@@ -534,9 +519,6 @@
     <t>cmip6.aerosol.key_properties.resolution.canonical_horizontal_resolution</t>
   </si>
   <si>
-    <t>180km or 1.875 degree</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.5.1.3 </t>
   </si>
   <si>
@@ -594,9 +576,6 @@
     <t>cmip6.aerosol.key_properties.tuning_applied.description</t>
   </si>
   <si>
-    <t>No tuning.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.6.1.2 </t>
   </si>
   <si>
@@ -660,10 +639,6 @@
     <t>cmip6.aerosol.grid.overview</t>
   </si>
   <si>
-    <t>Horizontal: Gaussian grids of 192 x 96 in longitude and latitude (approximately 180 km or 1.875 degree)
-Vertical: sigma-pressure hybrid coordinate with 80 vertical layers up to the 0.01 hPa lavel (same as the atmospheric model)</t>
-  </si>
-  <si>
     <t>2.1.1.3 *</t>
   </si>
   <si>
@@ -748,13 +723,6 @@
     <t>cmip6.aerosol.transport.overview</t>
   </si>
   <si>
-    <t>Grid-scale transport: 
-   Vertically conservative semi-Lagrangian scheme
-Subgrid-scale transport/mixing:
-   Vertical mixing due to turbulence
-   Vertical transport due to (deep) convection</t>
-  </si>
-  <si>
     <t>3.1.1.3 *</t>
   </si>
   <si>
@@ -767,15 +735,15 @@
     <t>cmip6.aerosol.transport.scheme</t>
   </si>
   <si>
+    <t>Uses atmospheric chemistry transport scheme</t>
+  </si>
+  <si>
+    <t>Specific transport scheme (eulerian)</t>
+  </si>
+  <si>
     <t>Specific transport scheme (semi-lagrangian)</t>
   </si>
   <si>
-    <t>Uses atmospheric chemistry transport scheme</t>
-  </si>
-  <si>
-    <t>Specific transport scheme (eulerian)</t>
-  </si>
-  <si>
     <t>Specific transport scheme (eulerian and semi-lagrangian)</t>
   </si>
   <si>
@@ -803,6 +771,9 @@
     <t>Gradients monotonicity</t>
   </si>
   <si>
+    <t>Other: gradients monotony</t>
+  </si>
+  <si>
     <t>3.1.1.5 *</t>
   </si>
   <si>
@@ -848,13 +819,6 @@
     <t>cmip6.aerosol.emissions.overview</t>
   </si>
   <si>
-    <t xml:space="preserve">Anthropogenic and biomass burning emissions (SO2, BC, OC) from the surface are obtained from the CMIP6 forcing data.
-Aircraft emissions (SO2, BC, OC) in 3-D grids are obtained from the CMIP6 forcing data.
-Sulfur species originating from natural source and sea salt and dust are interactively calculated in the model.
-SO2 originating from continuous volcanic eruptions are calculated from the Global Emissions Inventory Activity database SO2 emission inventory (Andres and Kasgnoc 1998). 
-</t>
-  </si>
-  <si>
     <t>4.1.1.3 *</t>
   </si>
   <si>
@@ -864,21 +828,21 @@
     <t>cmip6.aerosol.emissions.method</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Prescribed (climatology)</t>
+  </si>
+  <si>
+    <t>Prescribed CMIP6</t>
+  </si>
+  <si>
+    <t>Prescribed above surface</t>
+  </si>
+  <si>
     <t>Interactive</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Prescribed (climatology)</t>
-  </si>
-  <si>
-    <t>Prescribed CMIP6</t>
-  </si>
-  <si>
-    <t>Prescribed above surface</t>
-  </si>
-  <si>
     <t>Interactive above surface</t>
   </si>
   <si>
@@ -894,12 +858,12 @@
     <t>cmip6.aerosol.emissions.sources</t>
   </si>
   <si>
+    <t>Vegetation</t>
+  </si>
+  <si>
     <t>Volcanos</t>
   </si>
   <si>
-    <t>Vegetation</t>
-  </si>
-  <si>
     <t>Bare ground</t>
   </si>
   <si>
@@ -957,9 +921,6 @@
     <t>cmip6.aerosol.emissions.prescribed_climatology_emitted_species</t>
   </si>
   <si>
-    <t>SO2 from continuously degassing volcanoes</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.1.1.7 </t>
   </si>
   <si>
@@ -984,9 +945,6 @@
     <t>cmip6.aerosol.emissions.interactive_emitted_species</t>
   </si>
   <si>
-    <t>Mineral dust, sea salt, dimethyl sulfide from the ocean</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.1.1.9 </t>
   </si>
   <si>
@@ -1038,9 +996,6 @@
     <t>cmip6.aerosol.concentrations.overview</t>
   </si>
   <si>
-    <t>Aerosol concentrations are calculated by aerosol physical and chemical processes (e.g., emission, transport, diffusion, chemical reactions, and dry and wet depositions) in the aerosol model.</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.1.1.3 </t>
   </si>
   <si>
@@ -1119,10 +1074,6 @@
     <t>cmip6.aerosol.optical_radiative_properties.overview</t>
   </si>
   <si>
-    <t xml:space="preserve">Aerosol optical and radiative properties are calculated in the aerosol-radiation scheme in the atmospheric model using mass concentrations of aerosols, which are provided by the aerosol model. Descriptions shown in below are used in the atmospheric model.
-</t>
-  </si>
-  <si>
     <t>6.2.1</t>
   </si>
   <si>
@@ -1213,9 +1164,6 @@
     <t>cmip6.aerosol.optical_radiative_properties.mixtures.mixing_rule</t>
   </si>
   <si>
-    <t>Core-shell aerosol treatment for hydrophilic-BC/SO4 mixture, volume-weighted averaging for other aerosol species</t>
-  </si>
-  <si>
     <t>6.4.1</t>
   </si>
   <si>
@@ -1279,9 +1227,6 @@
     <t>cmip6.aerosol.optical_radiative_properties.radiative_scheme.overview</t>
   </si>
   <si>
-    <t>Radiation is calculated in the atmospheric model and there is no radiative scheme in the aerosol model. Descriptions shown in below are used in the atmospheric model.</t>
-  </si>
-  <si>
     <t>6.5.1.2 *</t>
   </si>
   <si>
@@ -1324,9 +1269,6 @@
     <t>cmip6.aerosol.optical_radiative_properties.cloud_interactions.overview</t>
   </si>
   <si>
-    <t>Aerosol-cloud interactions are calculated in the atmospheric model and there is no aerosol-cloud interaction scheme in the aerosol model. Descriptions shown in below are used in the atmospheric model.</t>
-  </si>
-  <si>
     <t>6.6.1.2 *</t>
   </si>
   <si>
@@ -1396,9 +1338,6 @@
     <t>cmip6.aerosol.model.name</t>
   </si>
   <si>
-    <t>MASINGAR</t>
-  </si>
-  <si>
     <t>7.1.1.2 *</t>
   </si>
   <si>
@@ -1408,7 +1347,8 @@
     <t>cmip6.aerosol.model.overview</t>
   </si>
   <si>
-    <t>MASINGAR (Model of Aerosol Species IN the Global AtmospheRe) treats the main five aerosol species (sulfates, organic aerosols, black carbon, sea salt, and mineral dust) and their precursors. It is developed in the Meteorological Research Institute (MRI) of Japan Meteorological Agency and used for the aerosol forecasting and climate researches. Log-normal size distributions are assumed for sulfates, BC, and OA, and size-bin method is used for the sea salt and mineral dust. Precursor gases of sulfates include dimethyl sulfide, sulfur dioxide, and sulfur trioxide, and oxidized to sulfates via gas- and aqueous-phase reactions. Oxidants of sulfur reactions include OH, NO2, O3, and provided by the chemistry model MRI-CCM2. BC and OA are separated into hydrophobic and hydrophilic particles and their conversion rate is calculated based on the abundance of sulfates. Aerosol concentrations are passed to the atmospheric model MRI-AGCM and aerosol-radiation and aerosol-cloud interactions are calculated in the atmospheric model. Deposition fluxes of the light absorbing aerosols (BC and mineral dust) are also passed to the atmospheric model and used for the calculation of snow darkening effect of snow and sea ice.</t>
+    <t>Coupling With: snow albedo on sea ice_x000D_
+Gas Phase Precursors: SO3</t>
   </si>
   <si>
     <t>7.1.1.3 *</t>
@@ -1474,15 +1414,15 @@
     <t>cmip6.aerosol.model.coupling</t>
   </si>
   <si>
+    <t>Clouds</t>
+  </si>
+  <si>
     <t>Radiation</t>
   </si>
   <si>
     <t>Land surface</t>
   </si>
   <si>
-    <t>Clouds</t>
-  </si>
-  <si>
     <t>Ocean</t>
   </si>
   <si>
@@ -1492,6 +1432,12 @@
     <t>Gas phase chemistry</t>
   </si>
   <si>
+    <t>Other: heterogeneouschemistry</t>
+  </si>
+  <si>
+    <t>Other: landsurface</t>
+  </si>
+  <si>
     <t>7.1.1.5 *</t>
   </si>
   <si>
@@ -1561,6 +1507,9 @@
     <t>cmip6.aerosol.model.bulk_scheme_species</t>
   </si>
   <si>
+    <t>Black carbon / soot</t>
+  </si>
+  <si>
     <t>Sulphate</t>
   </si>
   <si>
@@ -1574,9 +1523,6 @@
   </si>
   <si>
     <t>Organic</t>
-  </si>
-  <si>
-    <t>Black carbon / soot</t>
   </si>
   <si>
     <t>SOA (secondary organic aerosols)</t>
@@ -2575,7 +2521,7 @@
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
       <c r="B35" s="11">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
@@ -2657,16 +2603,14 @@
       </c>
     </row>
     <row r="51" spans="1:30" ht="24" customHeight="1">
-      <c r="B51" s="11" t="s">
-        <v>102</v>
-      </c>
+      <c r="B51" s="11"/>
     </row>
     <row r="53" spans="1:30" ht="24" customHeight="1">
       <c r="A53" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:30" ht="24" customHeight="1">
@@ -2674,10 +2618,10 @@
         <v>43</v>
       </c>
       <c r="B54" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:30" ht="24" customHeight="1">
@@ -2686,29 +2630,27 @@
       </c>
     </row>
     <row r="56" spans="1:30" ht="24" customHeight="1">
-      <c r="B56" s="11" t="s">
-        <v>107</v>
-      </c>
+      <c r="B56" s="11"/>
     </row>
     <row r="59" spans="1:30" ht="24" customHeight="1">
       <c r="A59" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:30" ht="24" customHeight="1">
       <c r="B60" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:30" ht="24" customHeight="1">
       <c r="A62" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:30" ht="24" customHeight="1">
@@ -2716,24 +2658,24 @@
         <v>60</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:30" ht="24" customHeight="1">
       <c r="B64" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AA64" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AB64" s="6" t="s">
         <v>115</v>
       </c>
       <c r="AC64" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AD64" s="6" t="s">
         <v>68</v>
@@ -2741,10 +2683,10 @@
     </row>
     <row r="66" spans="1:35" ht="24" customHeight="1">
       <c r="A66" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B66" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:35" ht="24" customHeight="1">
@@ -2752,23 +2694,21 @@
         <v>83</v>
       </c>
       <c r="B67" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C67" s="10" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="68" spans="1:35" ht="24" customHeight="1">
-      <c r="B68" s="11">
-        <v>900</v>
-      </c>
+      <c r="B68" s="11"/>
     </row>
     <row r="70" spans="1:35" ht="24" customHeight="1">
       <c r="A70" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:35" ht="24" customHeight="1">
@@ -2776,23 +2716,21 @@
         <v>83</v>
       </c>
       <c r="B71" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C71" s="10" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="72" spans="1:35" ht="24" customHeight="1">
-      <c r="B72" s="11">
-        <v>900</v>
-      </c>
+      <c r="B72" s="11"/>
     </row>
     <row r="74" spans="1:35" ht="24" customHeight="1">
       <c r="A74" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B74" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:35" ht="24" customHeight="1">
@@ -2800,10 +2738,10 @@
         <v>83</v>
       </c>
       <c r="B75" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C75" s="10" t="s">
         <v>128</v>
-      </c>
-      <c r="C75" s="10" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:35" ht="24" customHeight="1">
@@ -2813,10 +2751,10 @@
     </row>
     <row r="78" spans="1:35" ht="24" customHeight="1">
       <c r="A78" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B78" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:35" ht="24" customHeight="1">
@@ -2824,39 +2762,37 @@
         <v>60</v>
       </c>
       <c r="B79" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C79" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="C79" s="10" t="s">
+    </row>
+    <row r="80" spans="1:35" ht="24" customHeight="1">
+      <c r="B80" s="11"/>
+      <c r="AA80" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="80" spans="1:35" ht="24" customHeight="1">
-      <c r="B80" s="11" t="s">
+      <c r="AB80" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AA80" s="6" t="s">
+      <c r="AC80" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="AB80" s="6" t="s">
+      <c r="AD80" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="AC80" s="6" t="s">
+      <c r="AE80" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="AD80" s="6" t="s">
+      <c r="AF80" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="AE80" s="6" t="s">
+      <c r="AG80" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="AF80" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="AG80" s="6" t="s">
+      <c r="AH80" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="AH80" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="AI80" s="6" t="s">
         <v>68</v>
@@ -2864,10 +2800,10 @@
     </row>
     <row r="83" spans="1:3" ht="24" customHeight="1">
       <c r="A83" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="12" t="s">
         <v>142</v>
-      </c>
-      <c r="B83" s="12" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="24" customHeight="1">
@@ -2875,10 +2811,10 @@
     </row>
     <row r="86" spans="1:3" ht="24" customHeight="1">
       <c r="A86" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B86" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="24" customHeight="1">
@@ -2886,10 +2822,10 @@
         <v>43</v>
       </c>
       <c r="B87" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C87" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="24" customHeight="1">
@@ -2898,16 +2834,14 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="24" customHeight="1">
-      <c r="B89" s="11" t="s">
-        <v>148</v>
-      </c>
+      <c r="B89" s="11"/>
     </row>
     <row r="91" spans="1:3" ht="24" customHeight="1">
       <c r="A91" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="24" customHeight="1">
@@ -2915,10 +2849,10 @@
         <v>43</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="24" customHeight="1">
@@ -2927,16 +2861,14 @@
       </c>
     </row>
     <row r="94" spans="1:3" ht="24" customHeight="1">
-      <c r="B94" s="11" t="s">
-        <v>153</v>
-      </c>
+      <c r="B94" s="11"/>
     </row>
     <row r="96" spans="1:3" ht="24" customHeight="1">
       <c r="A96" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="24" customHeight="1">
@@ -2944,33 +2876,31 @@
         <v>83</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="24" customHeight="1">
-      <c r="B98" s="11">
-        <v>3600</v>
-      </c>
+      <c r="B98" s="11"/>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
       <c r="A101" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="24" customHeight="1">
       <c r="B102" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="24" customHeight="1">
       <c r="A104" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B104" s="9" t="s">
         <v>42</v>
@@ -2981,23 +2911,21 @@
         <v>43</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="24" customHeight="1">
-      <c r="B106" s="11" t="s">
-        <v>164</v>
-      </c>
+      <c r="B106" s="11"/>
     </row>
     <row r="108" spans="1:3" ht="24" customHeight="1">
       <c r="A108" s="9" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="24" customHeight="1">
@@ -3005,23 +2933,21 @@
         <v>43</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="24" customHeight="1">
-      <c r="B110" s="11" t="s">
-        <v>169</v>
-      </c>
+      <c r="B110" s="11"/>
     </row>
     <row r="112" spans="1:3" ht="24" customHeight="1">
       <c r="A112" s="9" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="24" customHeight="1">
@@ -3029,23 +2955,21 @@
         <v>83</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="24" customHeight="1">
-      <c r="B114" s="11">
-        <v>18432</v>
-      </c>
+      <c r="B114" s="11"/>
     </row>
     <row r="116" spans="1:3" ht="24" customHeight="1">
       <c r="A116" s="9" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="24" customHeight="1">
@@ -3053,23 +2977,21 @@
         <v>83</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="24" customHeight="1">
-      <c r="B118" s="11">
-        <v>80</v>
-      </c>
+      <c r="B118" s="11"/>
     </row>
     <row r="120" spans="1:3" ht="24" customHeight="1">
       <c r="A120" s="9" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="24" customHeight="1">
@@ -3077,36 +2999,34 @@
         <v>88</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="24" customHeight="1">
-      <c r="B122" s="11" t="b">
-        <v>0</v>
-      </c>
+      <c r="B122" s="11"/>
     </row>
     <row r="125" spans="1:3" ht="24" customHeight="1">
       <c r="A125" s="12" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="24" customHeight="1">
       <c r="B126" s="13" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="24" customHeight="1">
       <c r="A128" s="9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="24" customHeight="1">
@@ -3114,10 +3034,10 @@
         <v>43</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C129" s="10" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="24" customHeight="1">
@@ -3126,16 +3046,14 @@
       </c>
     </row>
     <row r="131" spans="1:3" ht="178" customHeight="1">
-      <c r="B131" s="11" t="s">
-        <v>189</v>
-      </c>
+      <c r="B131" s="11"/>
     </row>
     <row r="133" spans="1:3" ht="24" customHeight="1">
       <c r="A133" s="9" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1">
@@ -3143,10 +3061,10 @@
         <v>43</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C134" s="10" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="24" customHeight="1">
@@ -3159,10 +3077,10 @@
     </row>
     <row r="138" spans="1:3" ht="24" customHeight="1">
       <c r="A138" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="24" customHeight="1">
@@ -3170,10 +3088,10 @@
         <v>43</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="24" customHeight="1">
@@ -3186,10 +3104,10 @@
     </row>
     <row r="143" spans="1:3" ht="24" customHeight="1">
       <c r="A143" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1">
@@ -3197,10 +3115,10 @@
         <v>43</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="24" customHeight="1">
@@ -3276,20 +3194,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -3300,20 +3218,18 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11" t="s">
-        <v>164</v>
-      </c>
+      <c r="B6" s="11"/>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>53</v>
@@ -3324,10 +3240,10 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
@@ -3336,16 +3252,14 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11" t="s">
-        <v>211</v>
-      </c>
+      <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -3353,33 +3267,31 @@
         <v>88</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
-      <c r="B15" s="11" t="b">
-        <v>0</v>
-      </c>
+      <c r="B15" s="11"/>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
       <c r="B19" s="13" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>42</v>
@@ -3390,23 +3302,21 @@
         <v>43</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="24" customHeight="1">
-      <c r="B23" s="11" t="s">
-        <v>164</v>
-      </c>
+      <c r="B23" s="11"/>
     </row>
     <row r="25" spans="1:3" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="24" customHeight="1">
@@ -3414,23 +3324,21 @@
         <v>43</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="24" customHeight="1">
-      <c r="B27" s="11" t="s">
-        <v>169</v>
-      </c>
+      <c r="B27" s="11"/>
     </row>
     <row r="29" spans="1:3" ht="24" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="24" customHeight="1">
@@ -3438,23 +3346,21 @@
         <v>83</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="24" customHeight="1">
-      <c r="B31" s="11">
-        <v>18432</v>
-      </c>
+      <c r="B31" s="11"/>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="24" customHeight="1">
@@ -3462,23 +3368,21 @@
         <v>83</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
-      <c r="B35" s="11">
-        <v>80</v>
-      </c>
+      <c r="B35" s="11"/>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
@@ -3486,10 +3390,10 @@
         <v>88</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
@@ -3516,7 +3420,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD27"/>
+  <dimension ref="A1:XFD28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3530,20 +3434,20 @@
   <sheetData>
     <row r="1" spans="1:31" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -3554,10 +3458,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="24" customHeight="1">
@@ -3565,7 +3469,7 @@
     </row>
     <row r="8" spans="1:31" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>53</v>
@@ -3576,10 +3480,10 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="24" customHeight="1">
@@ -3588,16 +3492,14 @@
       </c>
     </row>
     <row r="11" spans="1:31" ht="178" customHeight="1">
-      <c r="B11" s="11" t="s">
-        <v>240</v>
-      </c>
+      <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:31" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="24" customHeight="1">
@@ -3605,38 +3507,36 @@
         <v>60</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="24" customHeight="1">
-      <c r="B15" s="11" t="s">
-        <v>245</v>
-      </c>
+      <c r="B15" s="11"/>
       <c r="AA15" s="6" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="AB15" s="6" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="AC15" s="6" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="AD15" s="6" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="AE15" s="6" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="24" customHeight="1">
@@ -3644,10 +3544,10 @@
         <v>60</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="24" customHeight="1">
@@ -3657,19 +3557,19 @@
     </row>
     <row r="20" spans="1:31" ht="24" customHeight="1">
       <c r="B20" s="11" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="AA20" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB20" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC20" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB20" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="AC20" s="6" t="s">
-        <v>254</v>
-      </c>
       <c r="AD20" s="6" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="AE20" s="6" t="s">
         <v>68</v>
@@ -3677,19 +3577,19 @@
     </row>
     <row r="21" spans="1:31" ht="24" customHeight="1">
       <c r="B21" s="11" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="AA21" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC21" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB21" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="AC21" s="6" t="s">
-        <v>254</v>
-      </c>
       <c r="AD21" s="6" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="AE21" s="6" t="s">
         <v>68</v>
@@ -3697,19 +3597,19 @@
     </row>
     <row r="22" spans="1:31" ht="24" customHeight="1">
       <c r="B22" s="11" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="AA22" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB22" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC22" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB22" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="AC22" s="6" t="s">
-        <v>254</v>
-      </c>
       <c r="AD22" s="6" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="AE22" s="6" t="s">
         <v>68</v>
@@ -3717,10 +3617,10 @@
     </row>
     <row r="24" spans="1:31" ht="24" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="24" customHeight="1">
@@ -3728,10 +3628,10 @@
         <v>60</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="24" customHeight="1">
@@ -3740,22 +3640,41 @@
       </c>
     </row>
     <row r="27" spans="1:31" ht="24" customHeight="1">
-      <c r="B27" s="11"/>
+      <c r="B27" s="11" t="s">
+        <v>254</v>
+      </c>
       <c r="AA27" s="6" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="AB27" s="6" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="AC27" s="6" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="AD27" s="6" t="s">
         <v>68</v>
       </c>
     </row>
+    <row r="28" spans="1:31" ht="24" customHeight="1">
+      <c r="B28" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA28" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB28" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AC28" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="AD28" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
       <formula1>AA15:AE15</formula1>
     </dataValidation>
@@ -3770,6 +3689,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
       <formula1>AA27:AD27</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28">
+      <formula1>AA28:AD28</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3778,7 +3700,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD54"/>
+  <dimension ref="A1:XFD49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3792,20 +3714,20 @@
   <sheetData>
     <row r="1" spans="1:33" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -3816,10 +3738,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="24" customHeight="1">
@@ -3827,7 +3749,7 @@
     </row>
     <row r="8" spans="1:33" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>53</v>
@@ -3838,10 +3760,10 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:33" ht="24" customHeight="1">
@@ -3850,16 +3772,14 @@
       </c>
     </row>
     <row r="11" spans="1:33" ht="178" customHeight="1">
-      <c r="B11" s="11" t="s">
-        <v>272</v>
-      </c>
+      <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:33" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="24" customHeight="1">
@@ -3867,10 +3787,10 @@
         <v>60</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="24" customHeight="1">
@@ -3879,26 +3799,24 @@
       </c>
     </row>
     <row r="16" spans="1:33" ht="24" customHeight="1">
-      <c r="B16" s="11" t="s">
-        <v>276</v>
-      </c>
+      <c r="B16" s="11"/>
       <c r="AA16" s="6" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="AB16" s="6" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="AC16" s="6" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="AD16" s="6" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="AE16" s="6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="AF16" s="6" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="AG16" s="6" t="s">
         <v>68</v>
@@ -3906,10 +3824,10 @@
     </row>
     <row r="18" spans="1:35" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:35" ht="24" customHeight="1">
@@ -3917,10 +3835,10 @@
         <v>60</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="24" customHeight="1">
@@ -3929,242 +3847,105 @@
       </c>
     </row>
     <row r="21" spans="1:35" ht="24" customHeight="1">
-      <c r="B21" s="11" t="s">
-        <v>286</v>
-      </c>
+      <c r="B21" s="11"/>
       <c r="AA21" s="6" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="AB21" s="6" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="AC21" s="6" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="AD21" s="6" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="AE21" s="6" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="AF21" s="6" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="AG21" s="6" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="AH21" s="6" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="AI21" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="24" customHeight="1">
-      <c r="B22" s="11" t="s">
+    <row r="23" spans="1:35" ht="24" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" ht="24" customHeight="1">
+      <c r="A24" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="AA22" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="AB22" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="AC22" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="AD22" s="6" t="s">
+      <c r="C24" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="AE22" s="6" t="s">
+    </row>
+    <row r="25" spans="1:35" ht="24" customHeight="1">
+      <c r="B25" s="11"/>
+      <c r="AA25" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="AF22" s="6" t="s">
+      <c r="AB25" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="AG22" s="6" t="s">
+      <c r="AC25" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="AH22" s="6" t="s">
+      <c r="AD25" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="AI22" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:35" ht="24" customHeight="1">
-      <c r="B23" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="AA23" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="AB23" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="AC23" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="AD23" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="AE23" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="AF23" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="AG23" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="AH23" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="AI23" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" ht="24" customHeight="1">
-      <c r="B24" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="AA24" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="AB24" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="AC24" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="AD24" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="AE24" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="AF24" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="AG24" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="AH24" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="AI24" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:35" ht="24" customHeight="1">
-      <c r="B25" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="AA25" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="AB25" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="AC25" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="AD25" s="6" t="s">
-        <v>289</v>
-      </c>
       <c r="AE25" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="AF25" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="AG25" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="AH25" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="AI25" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" ht="24" customHeight="1">
-      <c r="B26" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="AA26" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="AB26" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="AC26" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="AD26" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="AE26" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="AF26" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="AG26" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="AH26" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="AI26" s="6" t="s">
-        <v>68</v>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" ht="24" customHeight="1">
+      <c r="A27" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:35" ht="24" customHeight="1">
-      <c r="A28" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>295</v>
+      <c r="A28" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="1:35" ht="24" customHeight="1">
-      <c r="A29" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>297</v>
+      <c r="B29" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:35" ht="24" customHeight="1">
-      <c r="B30" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="AA30" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AB30" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="AC30" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="AD30" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="AE30" s="6" t="s">
-        <v>302</v>
-      </c>
+      <c r="B30" s="11"/>
     </row>
     <row r="32" spans="1:35" ht="24" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
@@ -4172,10 +3953,10 @@
         <v>43</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="24" customHeight="1">
@@ -4184,16 +3965,14 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
-      <c r="B35" s="11" t="s">
-        <v>307</v>
-      </c>
+      <c r="B35" s="11"/>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
@@ -4201,10 +3980,10 @@
         <v>43</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
@@ -4213,16 +3992,14 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="24" customHeight="1">
-      <c r="B40" s="11" t="s">
-        <v>277</v>
-      </c>
+      <c r="B40" s="11"/>
     </row>
     <row r="42" spans="1:3" ht="24" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
@@ -4230,10 +4007,10 @@
         <v>43</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="24" customHeight="1">
@@ -4242,16 +4019,14 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="24" customHeight="1">
-      <c r="B45" s="11" t="s">
-        <v>316</v>
-      </c>
+      <c r="B45" s="11"/>
     </row>
     <row r="47" spans="1:3" ht="24" customHeight="1">
       <c r="A47" s="9" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1">
@@ -4259,67 +4034,25 @@
         <v>43</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="24" customHeight="1">
-      <c r="B49" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="24" customHeight="1">
-      <c r="B50" s="11"/>
-    </row>
-    <row r="52" spans="1:3" ht="24" customHeight="1">
-      <c r="A52" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="24" customHeight="1">
-      <c r="A53" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="24" customHeight="1">
-      <c r="B54" s="11"/>
+        <v>314</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="24" customHeight="1">
+      <c r="B49" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
       <formula1>AA16:AG16</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
       <formula1>AA21:AI21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
-      <formula1>AA22:AI22</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
-      <formula1>AA23:AI23</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
-      <formula1>AA24:AI24</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
-      <formula1>AA25:AI25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26">
-      <formula1>AA26:AI26</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
-      <formula1>AA30:AE30</formula1>
+      <formula1>AA25:AE25</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4342,20 +4075,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -4366,10 +4099,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -4377,7 +4110,7 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>53</v>
@@ -4388,10 +4121,10 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
@@ -4400,16 +4133,14 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11" t="s">
-        <v>334</v>
-      </c>
+      <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -4417,10 +4148,10 @@
         <v>43</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
@@ -4430,15 +4161,15 @@
     </row>
     <row r="16" spans="1:3" ht="24" customHeight="1">
       <c r="B16" s="11" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
@@ -4446,10 +4177,10 @@
         <v>43</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="24" customHeight="1">
@@ -4458,16 +4189,14 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1">
-      <c r="B21" s="11" t="s">
-        <v>277</v>
-      </c>
+      <c r="B21" s="11"/>
     </row>
     <row r="23" spans="1:3" ht="24" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="24" customHeight="1">
@@ -4475,10 +4204,10 @@
         <v>43</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="24" customHeight="1">
@@ -4487,16 +4216,14 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="24" customHeight="1">
-      <c r="B26" s="11" t="s">
-        <v>277</v>
-      </c>
+      <c r="B26" s="11"/>
     </row>
     <row r="28" spans="1:3" ht="24" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="24" customHeight="1">
@@ -4504,10 +4231,10 @@
         <v>43</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="24" customHeight="1">
@@ -4539,20 +4266,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -4563,10 +4290,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -4574,7 +4301,7 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>53</v>
@@ -4585,10 +4312,10 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
@@ -4597,101 +4324,93 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11" t="s">
-        <v>361</v>
-      </c>
+      <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
-      <c r="B19" s="11">
-        <v>-0.79</v>
-      </c>
+      <c r="B19" s="11"/>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="24" customHeight="1">
-      <c r="B23" s="11">
-        <v>-0.0055</v>
-      </c>
+      <c r="B23" s="11"/>
     </row>
     <row r="25" spans="1:3" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="24" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="24" customHeight="1">
-      <c r="B27" s="11">
-        <v>-0.006</v>
-      </c>
+      <c r="B27" s="11"/>
     </row>
     <row r="30" spans="1:3" ht="24" customHeight="1">
       <c r="A30" s="12" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="24" customHeight="1">
@@ -4699,10 +4418,10 @@
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="24" customHeight="1">
@@ -4710,23 +4429,21 @@
         <v>88</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
-      <c r="B35" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="B35" s="11"/>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1">
@@ -4734,23 +4451,21 @@
         <v>88</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
-      <c r="B39" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="B39" s="11"/>
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
       <c r="A41" s="9" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="24" customHeight="1">
@@ -4758,36 +4473,34 @@
         <v>43</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
-      <c r="B43" s="11" t="s">
-        <v>392</v>
-      </c>
+      <c r="B43" s="11"/>
     </row>
     <row r="46" spans="1:3" ht="24" customHeight="1">
       <c r="A46" s="12" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="24" customHeight="1">
       <c r="B47" s="13" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="24" customHeight="1">
       <c r="A49" s="9" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="24" customHeight="1">
@@ -4795,23 +4508,21 @@
         <v>88</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="24" customHeight="1">
-      <c r="B51" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="B51" s="11"/>
     </row>
     <row r="53" spans="1:3" ht="24" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="24" customHeight="1">
@@ -4819,23 +4530,21 @@
         <v>88</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="24" customHeight="1">
-      <c r="B55" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="B55" s="11"/>
     </row>
     <row r="57" spans="1:3" ht="24" customHeight="1">
       <c r="A57" s="9" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="24" customHeight="1">
@@ -4843,33 +4552,31 @@
         <v>88</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="24" customHeight="1">
-      <c r="B59" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="B59" s="11"/>
     </row>
     <row r="62" spans="1:3" ht="24" customHeight="1">
       <c r="A62" s="12" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="24" customHeight="1">
       <c r="B63" s="13" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="24" customHeight="1">
       <c r="A65" s="9" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>53</v>
@@ -4880,10 +4587,10 @@
         <v>43</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="24" customHeight="1">
@@ -4892,16 +4599,14 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="178" customHeight="1">
-      <c r="B68" s="11" t="s">
-        <v>414</v>
-      </c>
+      <c r="B68" s="11"/>
     </row>
     <row r="70" spans="1:3" ht="24" customHeight="1">
       <c r="A70" s="9" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="24" customHeight="1">
@@ -4909,23 +4614,21 @@
         <v>83</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="24" customHeight="1">
-      <c r="B72" s="11">
-        <v>22</v>
-      </c>
+      <c r="B72" s="11"/>
     </row>
     <row r="74" spans="1:3" ht="24" customHeight="1">
       <c r="A74" s="9" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="24" customHeight="1">
@@ -4933,33 +4636,31 @@
         <v>83</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="24" customHeight="1">
-      <c r="B76" s="11">
-        <v>11</v>
-      </c>
+      <c r="B76" s="11"/>
     </row>
     <row r="79" spans="1:3" ht="24" customHeight="1">
       <c r="A79" s="12" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="24" customHeight="1">
       <c r="B80" s="13" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="24" customHeight="1">
       <c r="A82" s="9" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>53</v>
@@ -4970,10 +4671,10 @@
         <v>43</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="24" customHeight="1">
@@ -4982,16 +4683,14 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="178" customHeight="1">
-      <c r="B85" s="11" t="s">
-        <v>429</v>
-      </c>
+      <c r="B85" s="11"/>
     </row>
     <row r="87" spans="1:3" ht="24" customHeight="1">
       <c r="A87" s="9" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="24" customHeight="1">
@@ -4999,23 +4698,21 @@
         <v>88</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="24" customHeight="1">
-      <c r="B89" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="B89" s="11"/>
     </row>
     <row r="91" spans="1:3" ht="24" customHeight="1">
       <c r="A91" s="9" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="24" customHeight="1">
@@ -5023,23 +4720,21 @@
         <v>83</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="24" customHeight="1">
-      <c r="B93" s="11">
-        <v>0</v>
-      </c>
+      <c r="B93" s="11"/>
     </row>
     <row r="95" spans="1:3" ht="24" customHeight="1">
       <c r="A95" s="9" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="24" customHeight="1">
@@ -5047,23 +4742,21 @@
         <v>88</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="24" customHeight="1">
-      <c r="B97" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="B97" s="11"/>
     </row>
     <row r="99" spans="1:3" ht="24" customHeight="1">
       <c r="A99" s="9" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="24" customHeight="1">
@@ -5071,23 +4764,21 @@
         <v>88</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
-      <c r="B101" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="B101" s="11"/>
     </row>
     <row r="103" spans="1:3" ht="24" customHeight="1">
       <c r="A103" s="9" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="24" customHeight="1">
@@ -5095,10 +4786,10 @@
         <v>83</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
@@ -5161,7 +4852,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD53"/>
+  <dimension ref="A1:XFD55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5175,7 +4866,7 @@
   <sheetData>
     <row r="1" spans="1:39" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>5</v>
@@ -5183,12 +4874,12 @@
     </row>
     <row r="2" spans="1:39" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>42</v>
@@ -5199,20 +4890,18 @@
         <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="24" customHeight="1">
-      <c r="B6" s="11" t="s">
-        <v>453</v>
-      </c>
+      <c r="B6" s="11"/>
     </row>
     <row r="8" spans="1:39" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>53</v>
@@ -5223,10 +4912,10 @@
         <v>43</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="24" customHeight="1">
@@ -5236,15 +4925,15 @@
     </row>
     <row r="11" spans="1:39" ht="178" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13" spans="1:39" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
     </row>
     <row r="14" spans="1:39" ht="24" customHeight="1">
@@ -5252,10 +4941,10 @@
         <v>60</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15" spans="1:39" ht="24" customHeight="1">
@@ -5265,536 +4954,521 @@
     </row>
     <row r="16" spans="1:39" ht="24" customHeight="1">
       <c r="B16" s="11" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="AA16" s="6" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="AB16" s="6" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="AC16" s="6" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="AD16" s="6" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="AE16" s="6" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="AF16" s="6" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="AG16" s="6" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="AH16" s="6" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="AI16" s="6" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="AJ16" s="6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="AK16" s="6" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="AL16" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AM16" s="6" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:39" ht="24" customHeight="1">
       <c r="B17" s="11" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="AA17" s="6" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="AB17" s="6" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="AC17" s="6" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="AD17" s="6" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="AE17" s="6" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="AF17" s="6" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="AG17" s="6" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="AH17" s="6" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="AI17" s="6" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="AJ17" s="6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="AK17" s="6" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="AL17" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AM17" s="6" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="1:39" ht="24" customHeight="1">
       <c r="B18" s="11" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="AA18" s="6" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="AB18" s="6" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="AC18" s="6" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="AD18" s="6" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="AE18" s="6" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="AF18" s="6" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="AG18" s="6" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="AH18" s="6" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="AI18" s="6" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="AJ18" s="6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="AK18" s="6" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="AL18" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AM18" s="6" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="19" spans="1:39" ht="24" customHeight="1">
       <c r="B19" s="11" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="AA19" s="6" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="AB19" s="6" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="AC19" s="6" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="AD19" s="6" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="AE19" s="6" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="AF19" s="6" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="AG19" s="6" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="AH19" s="6" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="AI19" s="6" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="AJ19" s="6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="AK19" s="6" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="AL19" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AM19" s="6" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="20" spans="1:39" ht="24" customHeight="1">
       <c r="B20" s="11" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AA20" s="6" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="AB20" s="6" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="AC20" s="6" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="AD20" s="6" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="AE20" s="6" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="AF20" s="6" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="AG20" s="6" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="AH20" s="6" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="AI20" s="6" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="AJ20" s="6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="AK20" s="6" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="AL20" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AM20" s="6" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="21" spans="1:39" ht="24" customHeight="1">
       <c r="B21" s="11" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="AA21" s="6" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="AB21" s="6" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="AC21" s="6" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="AD21" s="6" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="AE21" s="6" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="AF21" s="6" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="AG21" s="6" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="AH21" s="6" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="AI21" s="6" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="AJ21" s="6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="AK21" s="6" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="AL21" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AM21" s="6" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="22" spans="1:39" ht="24" customHeight="1">
       <c r="B22" s="11" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="AA22" s="6" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="AB22" s="6" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="AC22" s="6" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="AD22" s="6" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="AE22" s="6" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="AF22" s="6" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="AG22" s="6" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="AH22" s="6" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="AI22" s="6" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="AJ22" s="6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="AK22" s="6" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="AL22" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AM22" s="6" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="23" spans="1:39" ht="24" customHeight="1">
       <c r="B23" s="11" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="AA23" s="6" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="AB23" s="6" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="AC23" s="6" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="AD23" s="6" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="AE23" s="6" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="AF23" s="6" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="AG23" s="6" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="AH23" s="6" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="AI23" s="6" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="AJ23" s="6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="AK23" s="6" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="AL23" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AM23" s="6" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="24" spans="1:39" ht="24" customHeight="1">
       <c r="B24" s="11" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="AA24" s="6" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="AB24" s="6" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="AC24" s="6" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="AD24" s="6" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="AE24" s="6" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="AF24" s="6" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="AG24" s="6" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="AH24" s="6" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="AI24" s="6" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="AJ24" s="6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="AK24" s="6" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="AL24" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AM24" s="6" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="25" spans="1:39" ht="24" customHeight="1">
       <c r="B25" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="AA25" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AB25" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AC25" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AD25" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AE25" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="AF25" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="AG25" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="AH25" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AI25" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AJ25" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK25" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="AL25" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="AM25" s="6" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" ht="24" customHeight="1">
+      <c r="A27" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" ht="24" customHeight="1">
+      <c r="A28" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" ht="24" customHeight="1">
+      <c r="B29" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" ht="24" customHeight="1">
+      <c r="B30" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="AA30" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="AB30" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="AC30" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="AD30" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="AE30" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AA25" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="AB25" s="6" t="s">
-        <v>464</v>
-      </c>
-      <c r="AC25" s="6" t="s">
-        <v>465</v>
-      </c>
-      <c r="AD25" s="6" t="s">
-        <v>466</v>
-      </c>
-      <c r="AE25" s="6" t="s">
+      <c r="AF30" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="AF25" s="6" t="s">
+      <c r="AG30" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="AG25" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="AH25" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="AI25" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AJ25" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="AK25" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AL25" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AM25" s="6" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="26" spans="1:39" ht="24" customHeight="1">
-      <c r="B26" s="11" t="s">
-        <v>470</v>
-      </c>
-      <c r="AA26" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="AB26" s="6" t="s">
-        <v>464</v>
-      </c>
-      <c r="AC26" s="6" t="s">
-        <v>465</v>
-      </c>
-      <c r="AD26" s="6" t="s">
-        <v>466</v>
-      </c>
-      <c r="AE26" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="AF26" s="6" t="s">
-        <v>468</v>
-      </c>
-      <c r="AG26" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="AH26" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="AI26" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="AJ26" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="AK26" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="AL26" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AM26" s="6" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="28" spans="1:39" ht="24" customHeight="1">
-      <c r="A28" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="29" spans="1:39" ht="24" customHeight="1">
-      <c r="A29" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="30" spans="1:39" ht="24" customHeight="1">
-      <c r="B30" s="10" t="s">
-        <v>28</v>
+      <c r="AH30" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:39" ht="24" customHeight="1">
       <c r="B31" s="11" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="AA31" s="6" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="AB31" s="6" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="AC31" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AD31" s="6" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="AE31" s="6" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="AF31" s="6" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
       <c r="AG31" s="6" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="AH31" s="6" t="s">
         <v>68</v>
@@ -5802,28 +5476,28 @@
     </row>
     <row r="32" spans="1:39" ht="24" customHeight="1">
       <c r="B32" s="11" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="AA32" s="6" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="AB32" s="6" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="AC32" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AD32" s="6" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="AE32" s="6" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="AF32" s="6" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
       <c r="AG32" s="6" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="AH32" s="6" t="s">
         <v>68</v>
@@ -5831,340 +5505,472 @@
     </row>
     <row r="33" spans="1:35" ht="24" customHeight="1">
       <c r="B33" s="11" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="AA33" s="6" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="AB33" s="6" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="AC33" s="6" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="AD33" s="6" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="AE33" s="6" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="AF33" s="6" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
       <c r="AG33" s="6" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="AH33" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:35" ht="24" customHeight="1">
-      <c r="B34" s="11" t="s">
+    <row r="35" spans="1:35" ht="24" customHeight="1">
+      <c r="A35" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" ht="24" customHeight="1">
+      <c r="A36" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" ht="24" customHeight="1">
+      <c r="B37" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" ht="24" customHeight="1">
+      <c r="B38" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="AA38" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AB38" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AC38" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD38" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AE38" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AF38" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="AG38" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="AA34" s="6" t="s">
+      <c r="AH38" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="AI38" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" ht="24" customHeight="1">
+      <c r="B39" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="AA39" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AB39" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AC39" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD39" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AE39" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="AB34" s="6" t="s">
+      <c r="AF39" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="AC34" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AD34" s="6" t="s">
+      <c r="AG39" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="AE34" s="6" t="s">
+      <c r="AH39" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="AF34" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="AG34" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="AH34" s="6" t="s">
+      <c r="AI39" s="6" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:35" ht="24" customHeight="1">
-      <c r="B35" s="11" t="s">
-        <v>483</v>
-      </c>
-      <c r="AA35" s="6" t="s">
-        <v>479</v>
-      </c>
-      <c r="AB35" s="6" t="s">
-        <v>480</v>
-      </c>
-      <c r="AC35" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="AD35" s="6" t="s">
-        <v>481</v>
-      </c>
-      <c r="AE35" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="AF35" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="AG35" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="AH35" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:35" ht="24" customHeight="1">
-      <c r="A37" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="38" spans="1:35" ht="24" customHeight="1">
-      <c r="A38" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>487</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="39" spans="1:35" ht="24" customHeight="1">
-      <c r="B39" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:35" ht="24" customHeight="1">
       <c r="B40" s="11" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="AA40" s="6" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="AB40" s="6" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="AC40" s="6" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="AD40" s="6" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="AE40" s="6" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="AF40" s="6" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="AG40" s="6" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="AH40" s="6" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="AI40" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:35" ht="24" customHeight="1">
-      <c r="B41" s="11" t="s">
+    <row r="42" spans="1:35" ht="24" customHeight="1">
+      <c r="A42" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" ht="24" customHeight="1">
+      <c r="A43" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" ht="24" customHeight="1">
+      <c r="B44" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" ht="24" customHeight="1">
+      <c r="B45" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="AA45" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="AB45" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="AC45" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="AD45" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" ht="24" customHeight="1">
+      <c r="B46" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="AA46" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="AB46" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="AC46" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="AD46" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35" ht="24" customHeight="1">
+      <c r="A48" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="AA41" s="6" t="s">
-        <v>489</v>
-      </c>
-      <c r="AB41" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="AC41" s="6" t="s">
+      <c r="B48" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="AD41" s="6" t="s">
+    </row>
+    <row r="49" spans="1:40" ht="24" customHeight="1">
+      <c r="A49" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="AE41" s="6" t="s">
+      <c r="C49" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="AF41" s="6" t="s">
+    </row>
+    <row r="50" spans="1:40" ht="24" customHeight="1">
+      <c r="B50" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:40" ht="24" customHeight="1">
+      <c r="B51" s="11" t="s">
         <v>494</v>
       </c>
-      <c r="AG41" s="6" t="s">
+      <c r="AA51" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="AH41" s="6" t="s">
+      <c r="AB51" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="AI41" s="6" t="s">
+      <c r="AC51" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="AD51" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="AE51" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF51" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="AG51" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="AH51" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="AI51" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="AJ51" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="AK51" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="AL51" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="AM51" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="AN51" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:35" ht="24" customHeight="1">
-      <c r="B42" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="AA42" s="6" t="s">
-        <v>489</v>
-      </c>
-      <c r="AB42" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="AC42" s="6" t="s">
-        <v>491</v>
-      </c>
-      <c r="AD42" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="AE42" s="6" t="s">
-        <v>493</v>
-      </c>
-      <c r="AF42" s="6" t="s">
+    <row r="52" spans="1:40" ht="24" customHeight="1">
+      <c r="B52" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="AA52" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="AB52" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="AC52" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="AD52" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="AE52" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF52" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="AG52" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="AG42" s="6" t="s">
+      <c r="AH52" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="AI52" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="AJ52" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="AK52" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="AL52" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="AM52" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="AN52" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:40" ht="24" customHeight="1">
+      <c r="B53" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="AA53" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="AH42" s="6" t="s">
+      <c r="AB53" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="AI42" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:35" ht="24" customHeight="1">
-      <c r="A44" s="9" t="s">
+      <c r="AC53" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="AD53" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="AE53" s="6" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="45" spans="1:35" ht="24" customHeight="1">
-      <c r="A45" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="10" t="s">
+      <c r="AF53" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="AG53" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="AH53" s="6" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="46" spans="1:35" ht="24" customHeight="1">
-      <c r="B46" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:35" ht="24" customHeight="1">
-      <c r="B47" s="11" t="s">
+      <c r="AI53" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="AA47" s="6" t="s">
+      <c r="AJ53" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="AB47" s="6" t="s">
+      <c r="AK53" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="AC47" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="AD47" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:35" ht="24" customHeight="1">
-      <c r="B48" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="AA48" s="6" t="s">
-        <v>502</v>
-      </c>
-      <c r="AB48" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="AC48" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="AD48" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:40" ht="24" customHeight="1">
-      <c r="A50" s="9" t="s">
+      <c r="AL53" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="AM53" s="6" t="s">
         <v>505</v>
-      </c>
-    </row>
-    <row r="51" spans="1:40" ht="24" customHeight="1">
-      <c r="A51" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="52" spans="1:40" ht="24" customHeight="1">
-      <c r="B52" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:40" ht="24" customHeight="1">
-      <c r="B53" s="11"/>
-      <c r="AA53" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="AB53" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="AC53" s="6" t="s">
-        <v>510</v>
-      </c>
-      <c r="AD53" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="AE53" s="6" t="s">
-        <v>511</v>
-      </c>
-      <c r="AF53" s="6" t="s">
-        <v>512</v>
-      </c>
-      <c r="AG53" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="AH53" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="AI53" s="6" t="s">
-        <v>515</v>
-      </c>
-      <c r="AJ53" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="AK53" s="6" t="s">
-        <v>517</v>
-      </c>
-      <c r="AL53" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="AM53" s="6" t="s">
-        <v>519</v>
       </c>
       <c r="AN53" s="6" t="s">
         <v>68</v>
       </c>
     </row>
+    <row r="54" spans="1:40" ht="24" customHeight="1">
+      <c r="B54" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="AA54" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="AB54" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="AC54" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="AD54" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="AE54" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF54" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="AG54" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="AH54" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="AI54" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="AJ54" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="AK54" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="AL54" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="AM54" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="AN54" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:40" ht="24" customHeight="1">
+      <c r="B55" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="AA55" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="AB55" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="AC55" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="AD55" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="AE55" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF55" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="AG55" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="AH55" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="AI55" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="AJ55" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="AK55" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="AL55" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="AM55" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="AN55" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="22">
+  <dataValidations count="24">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
       <formula1>AA16:AM16</formula1>
     </dataValidation>
@@ -6195,8 +6001,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
       <formula1>AA25:AM25</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26">
-      <formula1>AA26:AM26</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
+      <formula1>AA30:AH30</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
       <formula1>AA31:AH31</formula1>
@@ -6207,29 +6013,35 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33">
       <formula1>AA33:AH33</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34">
-      <formula1>AA34:AH34</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35">
-      <formula1>AA35:AH35</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38">
+      <formula1>AA38:AI38</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
+      <formula1>AA39:AI39</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40">
       <formula1>AA40:AI40</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41">
-      <formula1>AA41:AI41</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
-      <formula1>AA42:AI42</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47">
-      <formula1>AA47:AD47</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48">
-      <formula1>AA48:AD48</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45">
+      <formula1>AA45:AD45</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46">
+      <formula1>AA46:AD46</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51">
+      <formula1>AA51:AN51</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B52">
+      <formula1>AA52:AN52</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53">
       <formula1>AA53:AN53</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54">
+      <formula1>AA54:AN54</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
+      <formula1>AA55:AN55</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>